<commit_message>
updated the mean pc to be bw 0.73 to 0.76
</commit_message>
<xml_diff>
--- a/matlab/statistics/MeanDthdRanalysis.xlsx
+++ b/matlab/statistics/MeanDthdRanalysis.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1342DD10-FB47-4C80-8F30-71D84D81217F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B4AD9B-3117-4ABE-9620-6F670CA69A54}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
   <si>
     <t>Observation</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Conference</t>
+  </si>
+  <si>
+    <t>old73to75</t>
   </si>
 </sst>
 </file>
@@ -102,19 +105,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,18 +400,19 @@
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -423,10 +426,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -442,8 +448,11 @@
       <c r="E2" s="4">
         <v>150</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F2" s="1">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -459,8 +468,11 @@
       <c r="E3" s="4">
         <v>130</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F3" s="1">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -476,8 +488,11 @@
       <c r="E4" s="4">
         <v>166</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F4" s="1">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -493,8 +508,11 @@
       <c r="E5" s="4">
         <v>160</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F5" s="1">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -508,11 +526,14 @@
         <v>500</v>
       </c>
       <c r="E6" s="4">
+        <v>170</v>
+      </c>
+      <c r="F6" s="1">
         <v>172</v>
       </c>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -528,8 +549,11 @@
       <c r="E7" s="4">
         <v>166</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F7" s="1">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -545,8 +569,11 @@
       <c r="E8" s="4">
         <v>158</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F8" s="1">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -562,8 +589,11 @@
       <c r="E9" s="4">
         <v>121</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F9" s="1">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -579,8 +609,11 @@
       <c r="E10" s="4">
         <v>176</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F10" s="1">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -596,8 +629,11 @@
       <c r="E11" s="4">
         <v>147</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F11" s="1">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -611,10 +647,13 @@
         <v>500</v>
       </c>
       <c r="E12" s="4">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+        <v>246</v>
+      </c>
+      <c r="F12" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -630,80 +669,19 @@
       <c r="E13" s="4">
         <v>207</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-    </row>
-    <row r="15" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="J15" s="5"/>
+      <c r="F13" s="1">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
-      <c r="Q15" s="5"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-    </row>
-    <row r="17" spans="10:17" x14ac:dyDescent="0.35">
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-    </row>
-    <row r="18" spans="10:17" x14ac:dyDescent="0.35">
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-    </row>
-    <row r="19" spans="10:17" x14ac:dyDescent="0.35">
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-    </row>
-    <row r="20" spans="10:17" x14ac:dyDescent="0.35">
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-    </row>
-    <row r="21" spans="10:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
+    </row>
+    <row r="21" spans="12:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>

</xml_diff>